<commit_message>
[feat] special Ability System
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/GachaTable.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/GachaTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\UNITY_PROJECTS\ProjectI\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974B72B5-1810-418B-ADE3-F1EAC4A09F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C8A47-015E-46B3-8EC7-7E195A4353F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="3975" windowWidth="17655" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="2580" windowWidth="18270" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[feat] player stat ui
게이지, 아이템, HP 적용
</commit_message>
<xml_diff>
--- a/Util/ExcelToJsonWizard.v1.0.6/excel_files/GachaTable.xlsx
+++ b/Util/ExcelToJsonWizard.v1.0.6/excel_files/GachaTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\UNITY_PROJECTS\ProjectI\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F623041-EC0A-4F59-9DA2-19CBF87313A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C39C4EE-829E-41B2-98E7-7F4C429CFBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="3975" windowWidth="23460" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="23595" windowHeight="16605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>key</t>
   </si>
@@ -116,30 +116,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1008, 1025, 1129</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1005, 1006, 1010, 1013, 1428</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1007, 1051, 1080, 1109, 1165</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1004, 1012</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>OnlyRank1Pool</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1009, 1008, 1025, 1129</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>OnlyRank2Pool</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -156,19 +136,39 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1009, 1008, 1025, 1129, 1005, 1006, 1010, 1013, 1428</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1009, 1008, 1025, 1129, 1005, 1006, 1010, 1013, 1428, 1007, 1051, 1080, 1109, 1165</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1009, 1008, 1025, 1129, 1005, 1006, 1010, 1013, 1428, 1007, 1051, 1080, 1109, 1165, 1004, 1012</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1008, 1025, 1129, 1005, 1006, 1010, 1013, 1428, 1007, 1051, 1080, 1109, 1165, 1004, 1012</t>
+    <t>1009, 1036</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1008, 1025, 1129, 1167</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1005, 1006, 1010, 1013, 1428, 1275, 1330</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1007, 1051, 1080, 1109, 1165, 1265, 1390, 1224, 1153</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1004, 1012, 1360, 1149, 1114, 1105</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1009, 1036, 1008, 1025, 1129, 1167, 1005, 1006, 1010, 1013, 1428, 1275, 1330</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1009, 1036, 1008, 1025, 1129, 1167, 1005, 1006, 1010, 1013, 1428, 1275, 1330, 1007, 1051, 1080, 1109, 1165, 1265, 1390, 1224, 1153</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1008, 1025, 1129, 1167, 1005, 1006, 1010, 1013, 1428, 1275, 1330, 1007, 1051, 1080, 1109, 1165, 1265, 1390, 1224, 1153, 1004, 1012, 1360, 1149, 1114, 1105</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1005, 1006, 1010, 1013, 1428, 1275, 1330, 1007, 1051, 1080, 1109, 1165, 1265, 1390, 1224, 1153, 1004, 1012, 1360, 1149, 1114, 1105</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -617,13 +617,13 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -643,22 +643,22 @@
         <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2">
         <v>20</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -681,10 +681,10 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -695,22 +695,22 @@
         <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
         <v>40</v>
       </c>
       <c r="F7" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <v>20</v>
@@ -733,7 +733,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -744,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>100</v>
@@ -761,8 +761,8 @@
       <c r="G9" s="2">
         <v>0</v>
       </c>
-      <c r="H9" s="4">
-        <v>1009</v>
+      <c r="H9" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -796,7 +796,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -848,7 +848,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>